<commit_message>
Last update for r.192
</commit_message>
<xml_diff>
--- a/doc/std_ebrew.xlsx
+++ b/doc/std_ebrew.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="134">
   <si>
     <t>02. Fill MLT</t>
   </si>
@@ -70,9 +70,6 @@
     <t xml:space="preserve">   sp_idx++; timer1 = 0</t>
   </si>
   <si>
-    <t xml:space="preserve">            MLT empty (Vmlt &lt; VMLT_EMPTY)</t>
-  </si>
-  <si>
     <t>SP_BATCHES</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>04. Mash Timer Running</t>
   </si>
   <si>
-    <t xml:space="preserve">    ms[ms_idx].timer++</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -130,38 +124,192 @@
     <t>10. Wait for Boil</t>
   </si>
   <si>
-    <t xml:space="preserve">              timer5 = 0</t>
-  </si>
-  <si>
     <t>11. Now Boiling</t>
   </si>
   <si>
     <t>12. Boiling Finished, prepare Chiller</t>
   </si>
   <si>
-    <t xml:space="preserve">              Pump = On</t>
+    <t>05. Sparge Timer Running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 timer1++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        timer5++</t>
+  </si>
+  <si>
+    <t>06. Pump from MLT to Boil-Kettle</t>
+  </si>
+  <si>
+    <t>Not Used (Future Use)</t>
+  </si>
+  <si>
+    <t>03. Wait for MLT Temp.</t>
+  </si>
+  <si>
+    <t>15. Add Malt to MLT</t>
+  </si>
+  <si>
+    <t>16. Chill &amp; Pump to Fermentor</t>
+  </si>
+  <si>
+    <t>17. Finished!</t>
+  </si>
+  <si>
+    <t>ms[ms_idx].timer &gt;= time</t>
+  </si>
+  <si>
+    <t>ms_idx++</t>
+  </si>
+  <si>
+    <t>&amp;&amp; (ms_idx&gt;0)</t>
+  </si>
+  <si>
+    <t>14. Pump Pre-Fill</t>
+  </si>
+  <si>
+    <t>HLT Preheat Timer</t>
+  </si>
+  <si>
+    <t>sec.</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>Toffset</t>
+  </si>
+  <si>
+    <t>Preheat HLT to next temperature</t>
+  </si>
+  <si>
+    <t>Number of Sparge batches</t>
+  </si>
+  <si>
+    <t>Time to Rest during Sparging</t>
+  </si>
+  <si>
+    <t>min.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>BOIL_TIME (timer5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      ms[ms_idx].timer++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      mrest_tmr++</t>
+  </si>
+  <si>
+    <t>Mash Rest</t>
+  </si>
+  <si>
+    <t>SP_PREBOIL</t>
+  </si>
+  <si>
+    <t>SP_BOIL</t>
+  </si>
+  <si>
+    <t>tset_boil = SP_PREBOIL ; enable PID-Controller for Boil-Kettle</t>
+  </si>
+  <si>
+    <t>18. Mash Rest 5 Min.</t>
+  </si>
+  <si>
+    <t>!mash_rest || (mrest_tmr &gt; 5 min.)</t>
+  </si>
+  <si>
+    <t>1 = Mash rest 5 min. after malt is added</t>
+  </si>
+  <si>
+    <t>Preboil Setpoint Temp. for Boil-Kettle</t>
+  </si>
+  <si>
+    <t>Boil Setpoint Temp. for Boil-Kettle</t>
+  </si>
+  <si>
+    <t>Total boiling-time</t>
+  </si>
+  <si>
+    <t>if Tboil&gt;55</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>0x0200</t>
+  </si>
+  <si>
+    <t>0x0003</t>
+  </si>
+  <si>
+    <t>0x030B</t>
+  </si>
+  <si>
+    <t>0x0309</t>
+  </si>
+  <si>
+    <t>0x0141</t>
+  </si>
+  <si>
+    <t>0x0124</t>
+  </si>
+  <si>
+    <t>Main Brew-Pump</t>
+  </si>
+  <si>
+    <t>Pump 2 (in HLT)</t>
+  </si>
+  <si>
+    <t>Temperature offset for early start of mash timers</t>
+  </si>
+  <si>
+    <t>Toffset2</t>
+  </si>
+  <si>
+    <t>(Tmlt ≥ ms[ms_idx].temp + Toffset2)</t>
+  </si>
+  <si>
+    <t>BOIL_MIN_TEMP</t>
+  </si>
+  <si>
+    <t>Min. Boil-kettle Temp. to enable Gas-burner</t>
+  </si>
+  <si>
+    <t>Mash Settings</t>
+  </si>
+  <si>
+    <t>Options | Mash, Sparge &amp; Boil Settings</t>
+  </si>
+  <si>
+    <t>Boil Settings</t>
+  </si>
+  <si>
+    <t>Toffset0</t>
+  </si>
+  <si>
+    <t>19. Ready to add Malt</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">             </t>
+      <t xml:space="preserve">ms[ms_idx].timer </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Timeout (1 min.)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">             Temp. HLT Ok (thlt </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -170,27 +318,44 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> tset_hlt)</t>
+      <t xml:space="preserve"> (time - PREHEAT_TIME) &amp;&amp;</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">              ms_idx = 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             MLT Volume OK (Vmlt &gt; MASH_VOL)</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">   &amp;&amp; timer1 </t>
+      <t xml:space="preserve">    Vmlt - Vmlt_old </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">≥ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SP_VOL / SP_BATCHES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> (sp_idx == SP_BATCHES - 1) &amp;&amp; (Timer1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -199,21 +364,39 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> SP_TIME</t>
+      <t xml:space="preserve"> SP_TIME)</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">                     Vmlt_old - Vmlt </t>
+      <t xml:space="preserve">             ms[ms_idx].timer </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">≥ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">time &amp;&amp; (ms_idx </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -222,71 +405,21 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> SP_VOL / SP_BATCHES</t>
+      <t xml:space="preserve"> ms_total-1)</t>
     </r>
   </si>
   <si>
-    <t>05. Sparge Timer Running</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">    Vmlt - Vmlt_old </t>
+      <t xml:space="preserve">   &amp;&amp; timer1 </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">≥ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>SP_VOL / SP_BATCHES</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">                      Time-out2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                 timer1++</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">             ms[ms_idx].timer </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">≥ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">time &amp;&amp; (ms_idx </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -295,307 +428,13 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> ms_total-1)</t>
+      <t xml:space="preserve"> SP_TIME</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">            User selects 'Boiling Started'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            User selects 'Start Chilling'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            User selects 'Chilling Finished'</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ms[ms_idx].timer </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>≥</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (time - PREHEAT_TIME) &amp;&amp;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">                        timer5++</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            timer5 &gt; BOIL_TIME</t>
-  </si>
-  <si>
-    <t>06. Pump from MLT to Boil-Kettle</t>
-  </si>
-  <si>
-    <t>Not Used (Future Use)</t>
-  </si>
-  <si>
-    <t>03. Wait for MLT Temp.</t>
-  </si>
-  <si>
-    <t>15. Add Malt to MLT</t>
-  </si>
-  <si>
-    <t>16. Chill &amp; Pump to Fermentor</t>
-  </si>
-  <si>
-    <t>17. Finished!</t>
-  </si>
-  <si>
-    <t>ms[ms_idx].timer &gt;= time</t>
-  </si>
-  <si>
-    <t>ms_idx++</t>
-  </si>
-  <si>
-    <t>&amp;&amp; (ms_idx&gt;0)</t>
-  </si>
-  <si>
-    <t>14. Pump Pre-Fill</t>
-  </si>
-  <si>
-    <t>HLT Preheat Timer</t>
-  </si>
-  <si>
-    <t>sec.</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>Toffset</t>
-  </si>
-  <si>
-    <t>Preheat HLT to next temperature</t>
-  </si>
-  <si>
-    <t>Number of Sparge batches</t>
-  </si>
-  <si>
-    <t>Time to Rest during Sparging</t>
-  </si>
-  <si>
-    <t>min.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t>BOIL_TIME (timer5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             User enables PID Controller</t>
-  </si>
-  <si>
-    <t>User selects 'Malt added to MLT'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ms[ms_idx].timer++</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      mrest_tmr++</t>
-  </si>
-  <si>
-    <t>Mash Rest</t>
-  </si>
-  <si>
-    <t>SP_PREBOIL</t>
-  </si>
-  <si>
-    <t>SP_BOIL</t>
-  </si>
-  <si>
-    <t>tset_boil = SP_PREBOIL ; enable PID-Controller for Boil-Kettle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              tset_boil = SP_BOIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             tset_boil = 0 ; disable PID-Controller for Boil-Kettle</t>
-  </si>
-  <si>
-    <t>18. Mash Rest 5 Min.</t>
-  </si>
-  <si>
-    <t>!mash_rest || (mrest_tmr &gt; 5 min.)</t>
-  </si>
-  <si>
-    <t>1 = Mash rest 5 min. after malt is added</t>
-  </si>
-  <si>
-    <t>Preboil Setpoint Temp. for Boil-Kettle</t>
-  </si>
-  <si>
-    <t>Boil Setpoint Temp. for Boil-Kettle</t>
-  </si>
-  <si>
-    <t>Total boiling-time</t>
-  </si>
-  <si>
-    <t>if Tboil&gt;55</t>
-  </si>
-  <si>
-    <t>V8</t>
-  </si>
-  <si>
-    <t>P0</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>0x0000</t>
-  </si>
-  <si>
-    <t>0x0200</t>
-  </si>
-  <si>
-    <t>0x0003</t>
-  </si>
-  <si>
-    <t>0x030B</t>
-  </si>
-  <si>
-    <t>0x0309</t>
-  </si>
-  <si>
-    <t>0x0141</t>
-  </si>
-  <si>
-    <t>0x0124</t>
-  </si>
-  <si>
-    <t>Main Brew-Pump</t>
-  </si>
-  <si>
-    <t>Pump 2 (in HLT)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> (sp_idx == SP_BATCHES - 1) &amp;&amp; (Timer1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>≥</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SP_TIME)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">             HLT PID-Controller is disabled</t>
-  </si>
-  <si>
-    <t>Temperature offset to add to HLT Reference Temp.</t>
-  </si>
-  <si>
-    <t>Temperature offset for early start of mash timers</t>
-  </si>
-  <si>
-    <t>Toffset2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(Tmlt </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>≥</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ms[ms_idx].temp + Toffset2) &amp;&amp; (ms_idx==0)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                       Tset_hlt = ms[ms_idx].temp + </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="17"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1*To</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="17"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ffset; start timer</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tset_hlt = ms[ms_idx].temp + </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="17"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2*To</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="17"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ffset</t>
-    </r>
-  </si>
-  <si>
-    <t>(Tmlt ≥ ms[ms_idx].temp + Toffset2)</t>
   </si>
   <si>
     <r>
@@ -604,7 +443,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="17"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -613,7 +452,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="17"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -623,7 +462,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="17"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -632,7 +471,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="9"/>
         <color indexed="17"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -641,31 +480,218 @@
     </r>
   </si>
   <si>
-    <t>BOIL_MIN_TEMP</t>
-  </si>
-  <si>
-    <t>Min. Boil-kettle Temp. to enable Gas-burner</t>
-  </si>
-  <si>
-    <t>Mash Settings</t>
-  </si>
-  <si>
-    <t>Options | Mash, Sparge &amp; Boil Settings</t>
-  </si>
-  <si>
-    <t>Boil Settings</t>
-  </si>
-  <si>
-    <t>Toffset0</t>
-  </si>
-  <si>
-    <t>Temp. Offset to add to HLT Reference Temp. for dough-in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              Tset_hlt = ms[ms_idx].temp + Toffset0 ; Tset_Boil = 0</t>
-  </si>
-  <si>
-    <t>r1.92,  11-05-2018</t>
+    <r>
+      <t xml:space="preserve">Tset_hlt = ms[ms_idx].temp + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="17"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2*To</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="17"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ffset</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                       Tset_hlt = ms[ms_idx].temp + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="17"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1*To</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="17"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ffset; start timer</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> ms[ms_idx].timer++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               MLT empty (Vmlt &lt; VMLT_EMPTY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               timer5 &gt; BOIL_TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 timer5 = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              tset_boil = 0 ; disable PID-Controller for Boil-Kettle; brest_tmr = 0</t>
+  </si>
+  <si>
+    <t>brest_tmr++</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">               User selects 'Boiling Started' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>|| Tboil &gt; BOIL_DETECT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">               User selects 'Chilling Finished' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>|| flow_rate_cfc_low detected</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">               User selects 'Start Chilling' &amp;&amp; (!boil_rest || brest_tmr &gt; 5 min)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                        Vmlt_old - Vmlt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> SP_VOL / SP_BATCHES</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                       Time-out2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               HLT PID-Controller is disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               tset_boil = SP_BOIL</t>
+  </si>
+  <si>
+    <t>Boil Rest</t>
+  </si>
+  <si>
+    <t>1 = Let wort rest for 5 min. after boiling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Pump = On</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Timeout (1 min.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                Temp. HLT Ok (thlt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tset_hlt)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Tset_hlt = ms[ms_idx].temp + Toffset0 ; Tset_Boil = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 ms_idx = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 User enables PID Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 MLT Volume OK (Vmlt &gt; MASH_VOL)</t>
+  </si>
+  <si>
+    <t>User selects "Start adding malt to MLT"</t>
+  </si>
+  <si>
+    <t>User selects "Malt added to MLT"</t>
+  </si>
+  <si>
+    <t>Temp. Offset to compensate for mash dough-in</t>
+  </si>
+  <si>
+    <t>Temperature offset to compensate for HLT -&gt; MLT losses</t>
+  </si>
+  <si>
+    <t>Leave Pumps On</t>
+  </si>
+  <si>
+    <t>1 = Leave pumps on after MLT temperature is reached</t>
+  </si>
+  <si>
+    <t>Boil Detect</t>
+  </si>
+  <si>
+    <t>Lower-limit for detection of wort boiling</t>
+  </si>
+  <si>
+    <t>r1.92,  19-05-2018</t>
   </si>
 </sst>
 </file>
@@ -675,7 +701,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -718,22 +744,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="17"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -767,6 +780,62 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF008000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="17"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="17"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -960,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -973,16 +1042,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -999,16 +1065,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1105,10 +1169,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1117,7 +1181,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1126,6 +1190,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1140,9 +1223,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1336,15 +1416,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:colOff>409574</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>414617</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1355,8 +1435,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3971925" y="2286000"/>
-          <a:ext cx="0" cy="476250"/>
+          <a:off x="4566956" y="2686050"/>
+          <a:ext cx="5043" cy="294715"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2589,15 +2669,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1238250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>1238251</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>34488</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>44013</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2608,8 +2688,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1847850" y="2638425"/>
-          <a:ext cx="1857375" cy="9525"/>
+          <a:off x="2460079" y="2826298"/>
+          <a:ext cx="1860659" cy="9525"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2795,15 +2875,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1238250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>1231680</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>41057</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>1238249</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>147450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2814,29 +2894,34 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1847850" y="2638425"/>
-          <a:ext cx="9525" cy="609600"/>
+          <a:off x="2453508" y="2832867"/>
+          <a:ext cx="6569" cy="1748635"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
-          <a:gdLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 6897"/>
+            <a:gd name="connsiteY0" fmla="*/ 12144 h 12144"/>
+            <a:gd name="connsiteX1" fmla="*/ 6897 w 6897"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 12144"/>
+          </a:gdLst>
           <a:ahLst/>
           <a:cxnLst>
             <a:cxn ang="0">
-              <a:pos x="0" y="64"/>
+              <a:pos x="connsiteX0" y="connsiteY0"/>
             </a:cxn>
             <a:cxn ang="0">
-              <a:pos x="0" y="0"/>
+              <a:pos x="connsiteX1" y="connsiteY1"/>
             </a:cxn>
           </a:cxnLst>
-          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
-            <a:path w="1" h="64">
+            <a:path w="6897" h="12144">
               <a:moveTo>
-                <a:pt x="0" y="64"/>
+                <a:pt x="0" y="12144"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="6897" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2857,15 +2942,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>149444</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>41057</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>158969</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>2956</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2876,8 +2961,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3705225" y="2638425"/>
-          <a:ext cx="9525" cy="123825"/>
+          <a:off x="4327306" y="2832867"/>
+          <a:ext cx="9525" cy="290348"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4392,15 +4477,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
+      <xdr:colOff>399656</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>406226</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>13139</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>451945</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>6570</xdr:rowOff>
+      <xdr:rowOff>6569</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4411,29 +4496,34 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3973174" y="3461846"/>
-          <a:ext cx="45719" cy="814552"/>
+          <a:off x="4577518" y="3291034"/>
+          <a:ext cx="6570" cy="1313811"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
-          <a:gdLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1437"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 13423"/>
+            <a:gd name="connsiteX1" fmla="*/ 1437 w 1437"/>
+            <a:gd name="connsiteY1" fmla="*/ 13423 h 13423"/>
+          </a:gdLst>
           <a:ahLst/>
           <a:cxnLst>
             <a:cxn ang="0">
-              <a:pos x="0" y="0"/>
+              <a:pos x="connsiteX0" y="connsiteY0"/>
             </a:cxn>
             <a:cxn ang="0">
-              <a:pos x="0" y="34"/>
+              <a:pos x="connsiteX1" y="connsiteY1"/>
             </a:cxn>
           </a:cxnLst>
-          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:rect l="l" t="t" r="r" b="b"/>
           <a:pathLst>
-            <a:path w="1" h="34">
+            <a:path w="1437" h="13423">
               <a:moveTo>
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="34"/>
+                <a:pt x="1437" y="13423"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4559,13 +4649,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>841294</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>86591</xdr:rowOff>
+      <xdr:colOff>843831</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>843831</xdr:colOff>
+      <xdr:colOff>847397</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>6569</xdr:rowOff>
     </xdr:to>
@@ -4575,9 +4665,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7247537" y="3352305"/>
-          <a:ext cx="2537" cy="409835"/>
+        <a:xfrm flipH="1">
+          <a:off x="7866055" y="3612931"/>
+          <a:ext cx="3566" cy="335017"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4603,14 +4693,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>4329</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>72258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>854528</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>82261</xdr:rowOff>
+      <xdr:colOff>853966</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>75692</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4619,8 +4709,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="5191372" y="3347357"/>
-          <a:ext cx="2069399" cy="618"/>
+          <a:off x="5804726" y="3192517"/>
+          <a:ext cx="2071464" cy="3434"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5876,6 +5966,582 @@
           <a:round/>
           <a:headEnd type="none" w="med" len="med"/>
           <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>843831</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>78827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>847397</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="Rechte verbindingslijn met pijl 105"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="7866055" y="3199086"/>
+          <a:ext cx="3566" cy="249621"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1583121</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1234966</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>98534</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="TextBox 118"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5760983" y="2982310"/>
+          <a:ext cx="4204138" cy="236483"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="900" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>(Tmlt ≥ ms[ms_idx].temp + Toffset2) &amp;&amp; (ms_idx==0) &amp;&amp; leave_pump_on</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>729343</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="121" name="Straight Connector 120"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4898571" y="3265714"/>
+          <a:ext cx="5443" cy="696686"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="129" name="Straight Arrow Connector 128"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4898571" y="3967843"/>
+          <a:ext cx="2122715" cy="5443"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>706820</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>4506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>70756</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76764</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="130" name="TextBox 129"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4881491" y="3760077"/>
+          <a:ext cx="1595508" cy="235544"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="900" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>... &amp;&amp; !leave_pump_on</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100263</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>5013</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100263</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>60158</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="133" name="Straight Connector 132"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4281237" y="8988592"/>
+          <a:ext cx="0" cy="215566"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>416093</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>65171</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100263</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>65171</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="135" name="Straight Connector 134"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="3985461" y="9209171"/>
+          <a:ext cx="295776" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>411079</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>155408</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>416092</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>75198</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="142" name="Straight Connector 141"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipV="1">
+          <a:off x="3980447" y="8657724"/>
+          <a:ext cx="5013" cy="561474"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>411079</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100263</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="144" name="Straight Connector 143"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3980447" y="8662737"/>
+          <a:ext cx="300790" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100263</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>155408</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100263</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>10026</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="146" name="Straight Arrow Connector 145"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4281237" y="8657724"/>
+          <a:ext cx="0" cy="175460"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15040</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>5013</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>370974</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>11029</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="148" name="Line 67"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeShapeType="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2972803" y="8828171"/>
+          <a:ext cx="967539" cy="6016"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="150" name="Line 67"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeShapeType="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4638675" y="8753475"/>
+          <a:ext cx="647700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
     </xdr:sp>
@@ -6237,8 +6903,8 @@
   </sheetPr>
   <dimension ref="B2:Y78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6261,299 +6927,309 @@
   <sheetData>
     <row r="2" spans="3:24">
       <c r="C2" s="1"/>
-      <c r="W2" s="3" t="s">
-        <v>106</v>
-      </c>
+      <c r="W2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="X2" s="6"/>
     </row>
     <row r="3" spans="3:24">
       <c r="C3" s="8"/>
-      <c r="W3" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="W3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="X3" s="6"/>
     </row>
     <row r="4" spans="3:24">
       <c r="V4" s="3"/>
-      <c r="W4" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="W4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" s="6"/>
     </row>
     <row r="5" spans="3:24">
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W5" t="s">
-        <v>35</v>
-      </c>
+      <c r="C5" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="6"/>
     </row>
     <row r="6" spans="3:24">
-      <c r="C6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="W6" t="s">
-        <v>34</v>
-      </c>
+      <c r="C6" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" s="6"/>
     </row>
     <row r="7" spans="3:24">
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="V7" s="3"/>
-      <c r="W7" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="W7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="X7" s="6"/>
     </row>
     <row r="8" spans="3:24">
-      <c r="C8" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="W8" t="s">
-        <v>33</v>
-      </c>
+      <c r="C8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="X8" s="6"/>
     </row>
     <row r="9" spans="3:24">
-      <c r="F9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="W9" t="s">
-        <v>32</v>
-      </c>
+      <c r="F9" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="X9" s="6"/>
     </row>
     <row r="10" spans="3:24">
       <c r="D10" s="12"/>
-      <c r="F10" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="W10" t="s">
-        <v>31</v>
-      </c>
+      <c r="F10" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X10" s="6"/>
     </row>
     <row r="11" spans="3:24">
-      <c r="C11" s="20"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="4"/>
       <c r="F11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="W11" t="s">
-        <v>30</v>
-      </c>
+      <c r="W11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="X11" s="6"/>
     </row>
     <row r="12" spans="3:24">
-      <c r="F12" s="13" t="s">
-        <v>42</v>
+      <c r="F12" s="70" t="s">
+        <v>120</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="K12" s="64" t="s">
+      <c r="K12" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="L12" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="M12" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="N12" s="66" t="s">
-        <v>95</v>
-      </c>
-      <c r="O12" s="67" t="s">
+      <c r="L12" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="N12" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="O12" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="P12" s="67" t="s">
+      <c r="P12" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" s="66" t="s">
+      <c r="Q12" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="R12" s="67" t="s">
+      <c r="R12" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="S12" s="68" t="s">
+      <c r="S12" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="T12" s="68" t="s">
+      <c r="T12" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="U12" s="68" t="s">
+      <c r="U12" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="V12" s="66" t="s">
+      <c r="V12" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="W12" s="47"/>
+      <c r="W12" s="44"/>
       <c r="X12" s="5"/>
     </row>
     <row r="13" spans="3:24">
-      <c r="C13" s="14"/>
-      <c r="K13" s="52">
-        <v>0</v>
-      </c>
-      <c r="L13" s="41">
-        <v>0</v>
-      </c>
-      <c r="M13" s="42">
-        <v>0</v>
-      </c>
-      <c r="N13" s="35">
-        <v>0</v>
-      </c>
-      <c r="O13" s="36">
-        <v>0</v>
-      </c>
-      <c r="P13" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="36">
-        <v>0</v>
-      </c>
-      <c r="R13" s="36">
-        <v>0</v>
-      </c>
-      <c r="S13" s="36">
-        <v>0</v>
-      </c>
-      <c r="T13" s="36">
-        <v>0</v>
-      </c>
-      <c r="U13" s="49">
-        <v>0</v>
-      </c>
-      <c r="V13" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="W13" s="48"/>
+      <c r="C13" s="13"/>
+      <c r="K13" s="49">
+        <v>0</v>
+      </c>
+      <c r="L13" s="38">
+        <v>0</v>
+      </c>
+      <c r="M13" s="39">
+        <v>0</v>
+      </c>
+      <c r="N13" s="32">
+        <v>0</v>
+      </c>
+      <c r="O13" s="33">
+        <v>0</v>
+      </c>
+      <c r="P13" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="33">
+        <v>0</v>
+      </c>
+      <c r="R13" s="33">
+        <v>0</v>
+      </c>
+      <c r="S13" s="33">
+        <v>0</v>
+      </c>
+      <c r="T13" s="33">
+        <v>0</v>
+      </c>
+      <c r="U13" s="46">
+        <v>0</v>
+      </c>
+      <c r="V13" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="W13" s="45"/>
       <c r="X13" s="5"/>
     </row>
     <row r="14" spans="3:24">
-      <c r="C14" s="14"/>
-      <c r="F14" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="K14" s="54">
+      <c r="C14" s="13"/>
+      <c r="F14" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="51">
         <v>1</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="40">
         <v>1</v>
       </c>
-      <c r="M14" s="44">
-        <v>0</v>
-      </c>
-      <c r="N14" s="37">
-        <v>0</v>
-      </c>
-      <c r="O14" s="38">
-        <v>0</v>
-      </c>
-      <c r="P14" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="38">
-        <v>0</v>
-      </c>
-      <c r="R14" s="38">
-        <v>0</v>
-      </c>
-      <c r="S14" s="38">
-        <v>0</v>
-      </c>
-      <c r="T14" s="38">
-        <v>0</v>
-      </c>
-      <c r="U14" s="50">
-        <v>0</v>
-      </c>
-      <c r="V14" s="55" t="s">
-        <v>99</v>
-      </c>
-      <c r="W14" s="48"/>
+      <c r="M14" s="41">
+        <v>0</v>
+      </c>
+      <c r="N14" s="34">
+        <v>0</v>
+      </c>
+      <c r="O14" s="35">
+        <v>0</v>
+      </c>
+      <c r="P14" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="35">
+        <v>0</v>
+      </c>
+      <c r="R14" s="35">
+        <v>0</v>
+      </c>
+      <c r="S14" s="35">
+        <v>0</v>
+      </c>
+      <c r="T14" s="35">
+        <v>0</v>
+      </c>
+      <c r="U14" s="47">
+        <v>0</v>
+      </c>
+      <c r="V14" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="W14" s="45"/>
       <c r="X14" s="5"/>
     </row>
     <row r="15" spans="3:24">
-      <c r="C15" s="14"/>
-      <c r="F15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="54">
+      <c r="C15" s="13"/>
+      <c r="F15" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="K15" s="51">
         <v>14</v>
       </c>
-      <c r="L15" s="43">
-        <v>0</v>
-      </c>
-      <c r="M15" s="44">
-        <v>0</v>
-      </c>
-      <c r="N15" s="37">
-        <v>0</v>
-      </c>
-      <c r="O15" s="38">
-        <v>0</v>
-      </c>
-      <c r="P15" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="38">
-        <v>0</v>
-      </c>
-      <c r="R15" s="38">
-        <v>0</v>
-      </c>
-      <c r="S15" s="38">
-        <v>0</v>
-      </c>
-      <c r="T15" s="38">
+      <c r="L15" s="40">
+        <v>0</v>
+      </c>
+      <c r="M15" s="41">
+        <v>0</v>
+      </c>
+      <c r="N15" s="34">
+        <v>0</v>
+      </c>
+      <c r="O15" s="35">
+        <v>0</v>
+      </c>
+      <c r="P15" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="35">
+        <v>0</v>
+      </c>
+      <c r="R15" s="35">
+        <v>0</v>
+      </c>
+      <c r="S15" s="35">
+        <v>0</v>
+      </c>
+      <c r="T15" s="35">
         <v>1</v>
       </c>
-      <c r="U15" s="50">
+      <c r="U15" s="47">
         <v>1</v>
       </c>
-      <c r="V15" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="W15" s="48"/>
+      <c r="V15" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="W15" s="45"/>
       <c r="X15" s="5"/>
     </row>
     <row r="16" spans="3:24">
-      <c r="F16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="56">
+      <c r="F16" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="K16" s="53">
         <v>2</v>
       </c>
-      <c r="L16" s="45">
+      <c r="L16" s="42">
         <v>1</v>
       </c>
-      <c r="M16" s="46">
+      <c r="M16" s="43">
         <v>1</v>
       </c>
-      <c r="N16" s="39">
-        <v>0</v>
-      </c>
-      <c r="O16" s="40">
-        <v>0</v>
-      </c>
-      <c r="P16" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="40">
-        <v>0</v>
-      </c>
-      <c r="R16" s="40">
+      <c r="N16" s="36">
+        <v>0</v>
+      </c>
+      <c r="O16" s="37">
+        <v>0</v>
+      </c>
+      <c r="P16" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="37">
+        <v>0</v>
+      </c>
+      <c r="R16" s="37">
         <v>1</v>
       </c>
-      <c r="S16" s="40">
-        <v>0</v>
-      </c>
-      <c r="T16" s="40">
+      <c r="S16" s="37">
+        <v>0</v>
+      </c>
+      <c r="T16" s="37">
         <v>1</v>
       </c>
-      <c r="U16" s="51">
+      <c r="U16" s="48">
         <v>1</v>
       </c>
-      <c r="V16" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="W16" s="48"/>
+      <c r="V16" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="W16" s="45"/>
       <c r="X16" s="5"/>
     </row>
     <row r="17" spans="2:24">
@@ -6562,741 +7238,767 @@
       <c r="F17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K17" s="58">
+      <c r="K17" s="55">
         <v>3</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="38">
         <v>1</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17" s="39">
         <v>1</v>
       </c>
-      <c r="N17" s="35">
-        <v>0</v>
-      </c>
-      <c r="O17" s="36">
-        <v>0</v>
-      </c>
-      <c r="P17" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="36">
-        <v>0</v>
-      </c>
-      <c r="R17" s="36">
+      <c r="N17" s="32">
+        <v>0</v>
+      </c>
+      <c r="O17" s="33">
+        <v>0</v>
+      </c>
+      <c r="P17" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="33">
+        <v>0</v>
+      </c>
+      <c r="R17" s="33">
         <v>1</v>
       </c>
-      <c r="S17" s="36">
-        <v>0</v>
-      </c>
-      <c r="T17" s="36">
-        <v>0</v>
-      </c>
-      <c r="U17" s="49">
+      <c r="S17" s="33">
+        <v>0</v>
+      </c>
+      <c r="T17" s="33">
+        <v>0</v>
+      </c>
+      <c r="U17" s="46">
         <v>1</v>
       </c>
-      <c r="V17" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="W17" s="48"/>
+      <c r="V17" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="W17" s="45"/>
       <c r="X17" s="5"/>
     </row>
     <row r="18" spans="2:24">
       <c r="C18" s="8"/>
       <c r="D18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>44</v>
+      <c r="F18" s="69" t="s">
+        <v>124</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="K18" s="59">
-        <v>15</v>
-      </c>
-      <c r="L18" s="43">
-        <v>0</v>
-      </c>
-      <c r="M18" s="44">
-        <v>0</v>
-      </c>
-      <c r="N18" s="37">
-        <v>0</v>
-      </c>
-      <c r="O18" s="38">
-        <v>0</v>
-      </c>
-      <c r="P18" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="38">
-        <v>0</v>
-      </c>
-      <c r="R18" s="38">
-        <v>0</v>
-      </c>
-      <c r="S18" s="38">
-        <v>0</v>
-      </c>
-      <c r="T18" s="38">
-        <v>0</v>
-      </c>
-      <c r="U18" s="50">
-        <v>0</v>
-      </c>
-      <c r="V18" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="W18" s="48"/>
+      <c r="K18" s="56">
+        <v>19</v>
+      </c>
+      <c r="L18" s="40">
+        <v>1</v>
+      </c>
+      <c r="M18" s="41">
+        <v>1</v>
+      </c>
+      <c r="N18" s="34">
+        <v>0</v>
+      </c>
+      <c r="O18" s="35">
+        <v>0</v>
+      </c>
+      <c r="P18" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="35">
+        <v>0</v>
+      </c>
+      <c r="R18" s="35">
+        <v>1</v>
+      </c>
+      <c r="S18" s="35">
+        <v>0</v>
+      </c>
+      <c r="T18" s="35">
+        <v>0</v>
+      </c>
+      <c r="U18" s="47">
+        <v>1</v>
+      </c>
+      <c r="V18" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="W18" s="45"/>
       <c r="X18" s="5"/>
     </row>
     <row r="19" spans="2:24">
       <c r="C19" s="8"/>
       <c r="F19" s="8"/>
-      <c r="K19" s="59">
-        <v>18</v>
-      </c>
-      <c r="L19" s="43">
-        <v>0</v>
-      </c>
-      <c r="M19" s="44">
-        <v>0</v>
-      </c>
-      <c r="N19" s="37">
-        <v>0</v>
-      </c>
-      <c r="O19" s="38">
-        <v>0</v>
-      </c>
-      <c r="P19" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="38">
-        <v>0</v>
-      </c>
-      <c r="R19" s="38">
-        <v>0</v>
-      </c>
-      <c r="S19" s="38">
-        <v>0</v>
-      </c>
-      <c r="T19" s="38">
-        <v>0</v>
-      </c>
-      <c r="U19" s="50">
-        <v>0</v>
-      </c>
-      <c r="V19" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="W19" s="48"/>
+      <c r="K19" s="56">
+        <v>15</v>
+      </c>
+      <c r="L19" s="40">
+        <v>0</v>
+      </c>
+      <c r="M19" s="41">
+        <v>0</v>
+      </c>
+      <c r="N19" s="34">
+        <v>0</v>
+      </c>
+      <c r="O19" s="35">
+        <v>0</v>
+      </c>
+      <c r="P19" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="35">
+        <v>0</v>
+      </c>
+      <c r="R19" s="35">
+        <v>0</v>
+      </c>
+      <c r="S19" s="35">
+        <v>0</v>
+      </c>
+      <c r="T19" s="35">
+        <v>0</v>
+      </c>
+      <c r="U19" s="47">
+        <v>0</v>
+      </c>
+      <c r="V19" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="W19" s="45"/>
       <c r="X19" s="5"/>
     </row>
     <row r="20" spans="2:24">
-      <c r="F20" s="8"/>
-      <c r="K20" s="59">
-        <v>4</v>
-      </c>
-      <c r="L20" s="43">
-        <v>1</v>
-      </c>
-      <c r="M20" s="44">
-        <v>1</v>
-      </c>
-      <c r="N20" s="37">
-        <v>0</v>
-      </c>
-      <c r="O20" s="38">
-        <v>0</v>
-      </c>
-      <c r="P20" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="38">
-        <v>0</v>
-      </c>
-      <c r="R20" s="38">
-        <v>1</v>
-      </c>
-      <c r="S20" s="38">
-        <v>0</v>
-      </c>
-      <c r="T20" s="38">
-        <v>0</v>
-      </c>
-      <c r="U20" s="50">
-        <v>1</v>
-      </c>
-      <c r="V20" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="W20" s="48"/>
+      <c r="F20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="56">
+        <v>18</v>
+      </c>
+      <c r="L20" s="40">
+        <v>0</v>
+      </c>
+      <c r="M20" s="41">
+        <v>0</v>
+      </c>
+      <c r="N20" s="34">
+        <v>0</v>
+      </c>
+      <c r="O20" s="35">
+        <v>0</v>
+      </c>
+      <c r="P20" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="35">
+        <v>0</v>
+      </c>
+      <c r="R20" s="35">
+        <v>0</v>
+      </c>
+      <c r="S20" s="35">
+        <v>0</v>
+      </c>
+      <c r="T20" s="35">
+        <v>0</v>
+      </c>
+      <c r="U20" s="47">
+        <v>0</v>
+      </c>
+      <c r="V20" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="W20" s="45"/>
       <c r="X20" s="5"/>
     </row>
     <row r="21" spans="2:24">
       <c r="C21" s="1"/>
       <c r="F21" s="8"/>
-      <c r="K21" s="60">
-        <v>13</v>
-      </c>
-      <c r="L21" s="45">
+      <c r="K21" s="56">
+        <v>4</v>
+      </c>
+      <c r="L21" s="40">
         <v>1</v>
       </c>
-      <c r="M21" s="46">
-        <v>0</v>
-      </c>
-      <c r="N21" s="39">
-        <v>0</v>
-      </c>
-      <c r="O21" s="40">
-        <v>0</v>
-      </c>
-      <c r="P21" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="40">
-        <v>0</v>
-      </c>
-      <c r="R21" s="40">
-        <v>0</v>
-      </c>
-      <c r="S21" s="40">
-        <v>0</v>
-      </c>
-      <c r="T21" s="40">
-        <v>0</v>
-      </c>
-      <c r="U21" s="51">
-        <v>0</v>
-      </c>
-      <c r="V21" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="W21" s="48"/>
+      <c r="M21" s="41">
+        <v>1</v>
+      </c>
+      <c r="N21" s="34">
+        <v>0</v>
+      </c>
+      <c r="O21" s="35">
+        <v>0</v>
+      </c>
+      <c r="P21" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="35">
+        <v>0</v>
+      </c>
+      <c r="R21" s="35">
+        <v>1</v>
+      </c>
+      <c r="S21" s="35">
+        <v>0</v>
+      </c>
+      <c r="T21" s="35">
+        <v>0</v>
+      </c>
+      <c r="U21" s="47">
+        <v>1</v>
+      </c>
+      <c r="V21" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="W21" s="45"/>
       <c r="X21" s="5"/>
     </row>
     <row r="22" spans="2:24">
       <c r="C22" s="8"/>
-      <c r="F22" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="K22" s="61">
-        <v>5</v>
-      </c>
-      <c r="L22" s="41">
+      <c r="I22" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="K22" s="57">
+        <v>13</v>
+      </c>
+      <c r="L22" s="42">
         <v>1</v>
       </c>
-      <c r="M22" s="42">
-        <v>1</v>
-      </c>
-      <c r="N22" s="35">
-        <v>0</v>
-      </c>
-      <c r="O22" s="36">
-        <v>0</v>
-      </c>
-      <c r="P22" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="36">
-        <v>0</v>
-      </c>
-      <c r="R22" s="36">
-        <v>1</v>
-      </c>
-      <c r="S22" s="36">
-        <v>0</v>
-      </c>
-      <c r="T22" s="36">
-        <v>0</v>
-      </c>
-      <c r="U22" s="49">
-        <v>1</v>
-      </c>
-      <c r="V22" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="W22" s="48"/>
+      <c r="M22" s="43">
+        <v>0</v>
+      </c>
+      <c r="N22" s="36">
+        <v>0</v>
+      </c>
+      <c r="O22" s="37">
+        <v>0</v>
+      </c>
+      <c r="P22" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="37">
+        <v>0</v>
+      </c>
+      <c r="R22" s="37">
+        <v>0</v>
+      </c>
+      <c r="S22" s="37">
+        <v>0</v>
+      </c>
+      <c r="T22" s="37">
+        <v>0</v>
+      </c>
+      <c r="U22" s="48">
+        <v>0</v>
+      </c>
+      <c r="V22" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="W22" s="45"/>
       <c r="X22" s="5"/>
     </row>
     <row r="23" spans="2:24">
-      <c r="B23" s="1" t="s">
-        <v>64</v>
+      <c r="B23" s="69" t="s">
+        <v>46</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="12" t="s">
-        <v>115</v>
+      <c r="D23" s="72" t="s">
+        <v>87</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K23" s="62">
-        <v>6</v>
-      </c>
-      <c r="L23" s="43">
-        <v>0</v>
-      </c>
-      <c r="M23" s="44">
+      <c r="G23" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="K23" s="58">
+        <v>5</v>
+      </c>
+      <c r="L23" s="38">
         <v>1</v>
       </c>
-      <c r="N23" s="37">
-        <v>0</v>
-      </c>
-      <c r="O23" s="38">
+      <c r="M23" s="39">
         <v>1</v>
       </c>
-      <c r="P23" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="38">
-        <v>0</v>
-      </c>
-      <c r="R23" s="38">
-        <v>0</v>
-      </c>
-      <c r="S23" s="38">
-        <v>0</v>
-      </c>
-      <c r="T23" s="38">
-        <v>0</v>
-      </c>
-      <c r="U23" s="50">
+      <c r="N23" s="32">
+        <v>0</v>
+      </c>
+      <c r="O23" s="33">
+        <v>0</v>
+      </c>
+      <c r="P23" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="33">
+        <v>0</v>
+      </c>
+      <c r="R23" s="33">
         <v>1</v>
       </c>
-      <c r="V23" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="W23" s="48"/>
+      <c r="S23" s="33">
+        <v>0</v>
+      </c>
+      <c r="T23" s="33">
+        <v>0</v>
+      </c>
+      <c r="U23" s="46">
+        <v>1</v>
+      </c>
+      <c r="V23" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="W23" s="45"/>
       <c r="X23" s="5"/>
     </row>
     <row r="24" spans="2:24">
-      <c r="C24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>66</v>
+      <c r="C24" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>48</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="16"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="62">
-        <v>8</v>
-      </c>
-      <c r="L24" s="43">
-        <v>0</v>
-      </c>
-      <c r="M24" s="44">
-        <v>0</v>
-      </c>
-      <c r="N24" s="37">
-        <v>0</v>
-      </c>
-      <c r="O24" s="38">
-        <v>0</v>
-      </c>
-      <c r="P24" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="38">
-        <v>0</v>
-      </c>
-      <c r="R24" s="38">
-        <v>0</v>
-      </c>
-      <c r="S24" s="38">
-        <v>0</v>
-      </c>
-      <c r="T24" s="38">
-        <v>0</v>
-      </c>
-      <c r="U24" s="50">
-        <v>0</v>
-      </c>
-      <c r="V24" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="W24" s="48"/>
+      <c r="K24" s="59">
+        <v>6</v>
+      </c>
+      <c r="L24" s="40">
+        <v>0</v>
+      </c>
+      <c r="M24" s="41">
+        <v>1</v>
+      </c>
+      <c r="N24" s="34">
+        <v>0</v>
+      </c>
+      <c r="O24" s="35">
+        <v>1</v>
+      </c>
+      <c r="P24" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="35">
+        <v>0</v>
+      </c>
+      <c r="R24" s="35">
+        <v>0</v>
+      </c>
+      <c r="S24" s="35">
+        <v>0</v>
+      </c>
+      <c r="T24" s="35">
+        <v>0</v>
+      </c>
+      <c r="U24" s="47">
+        <v>1</v>
+      </c>
+      <c r="V24" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="W24" s="45"/>
       <c r="X24" s="5"/>
     </row>
     <row r="25" spans="2:24">
-      <c r="B25" s="8" t="s">
-        <v>114</v>
+      <c r="B25" s="79" t="s">
+        <v>101</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="24"/>
-      <c r="K25" s="63">
-        <v>7</v>
-      </c>
-      <c r="L25" s="45">
-        <v>1</v>
-      </c>
-      <c r="M25" s="46">
-        <v>1</v>
-      </c>
-      <c r="N25" s="39">
-        <v>0</v>
-      </c>
-      <c r="O25" s="40">
-        <v>0</v>
-      </c>
-      <c r="P25" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="40">
-        <v>0</v>
-      </c>
-      <c r="R25" s="40">
-        <v>1</v>
-      </c>
-      <c r="S25" s="40">
-        <v>0</v>
-      </c>
-      <c r="T25" s="40">
-        <v>1</v>
-      </c>
-      <c r="U25" s="51">
-        <v>1</v>
-      </c>
-      <c r="V25" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="W25" s="48"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="23"/>
+      <c r="K25" s="59">
+        <v>8</v>
+      </c>
+      <c r="L25" s="40">
+        <v>0</v>
+      </c>
+      <c r="M25" s="41">
+        <v>0</v>
+      </c>
+      <c r="N25" s="34">
+        <v>0</v>
+      </c>
+      <c r="O25" s="35">
+        <v>0</v>
+      </c>
+      <c r="P25" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="35">
+        <v>0</v>
+      </c>
+      <c r="R25" s="35">
+        <v>0</v>
+      </c>
+      <c r="S25" s="35">
+        <v>0</v>
+      </c>
+      <c r="T25" s="35">
+        <v>0</v>
+      </c>
+      <c r="U25" s="47">
+        <v>0</v>
+      </c>
+      <c r="V25" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="W25" s="45"/>
       <c r="X25" s="5"/>
     </row>
     <row r="26" spans="2:24">
-      <c r="F26" s="27"/>
-      <c r="G26" s="29" t="s">
+      <c r="F26" s="25"/>
+      <c r="G26" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="H26" s="26"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="60">
+        <v>7</v>
+      </c>
+      <c r="L26" s="42">
+        <v>1</v>
+      </c>
+      <c r="M26" s="43">
+        <v>1</v>
+      </c>
+      <c r="N26" s="36">
+        <v>0</v>
+      </c>
+      <c r="O26" s="37">
+        <v>0</v>
+      </c>
+      <c r="P26" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="37">
+        <v>0</v>
+      </c>
+      <c r="R26" s="37">
+        <v>1</v>
+      </c>
+      <c r="S26" s="37">
+        <v>0</v>
+      </c>
+      <c r="T26" s="37">
+        <v>1</v>
+      </c>
+      <c r="U26" s="48">
+        <v>1</v>
+      </c>
+      <c r="V26" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="H26" s="29"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="52">
-        <v>9</v>
-      </c>
-      <c r="L26" s="41">
-        <v>0</v>
-      </c>
-      <c r="M26" s="42">
-        <v>1</v>
-      </c>
-      <c r="N26" s="35">
-        <v>0</v>
-      </c>
-      <c r="O26" s="36">
-        <v>1</v>
-      </c>
-      <c r="P26" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="36">
-        <v>0</v>
-      </c>
-      <c r="R26" s="36">
-        <v>0</v>
-      </c>
-      <c r="S26" s="36">
-        <v>0</v>
-      </c>
-      <c r="T26" s="36">
-        <v>0</v>
-      </c>
-      <c r="U26" s="49">
-        <v>1</v>
-      </c>
-      <c r="V26" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="W26" s="48"/>
+      <c r="W26" s="45"/>
       <c r="X26" s="5"/>
     </row>
     <row r="27" spans="2:24">
-      <c r="B27" s="8" t="s">
-        <v>27</v>
+      <c r="B27" s="79" t="s">
+        <v>25</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="K27" s="54">
-        <v>10</v>
-      </c>
-      <c r="L27" s="43">
-        <v>0</v>
-      </c>
-      <c r="M27" s="44">
-        <v>0</v>
-      </c>
-      <c r="N27" s="37">
-        <v>0</v>
-      </c>
-      <c r="O27" s="38">
-        <v>0</v>
-      </c>
-      <c r="P27" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="38">
-        <v>0</v>
-      </c>
-      <c r="R27" s="38">
-        <v>0</v>
-      </c>
-      <c r="S27" s="38">
-        <v>0</v>
-      </c>
-      <c r="T27" s="38">
-        <v>0</v>
-      </c>
-      <c r="U27" s="50">
-        <v>0</v>
-      </c>
-      <c r="V27" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="W27" s="48"/>
+      <c r="K27" s="49">
+        <v>9</v>
+      </c>
+      <c r="L27" s="38">
+        <v>0</v>
+      </c>
+      <c r="M27" s="39">
+        <v>1</v>
+      </c>
+      <c r="N27" s="32">
+        <v>0</v>
+      </c>
+      <c r="O27" s="33">
+        <v>1</v>
+      </c>
+      <c r="P27" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="33">
+        <v>0</v>
+      </c>
+      <c r="R27" s="33">
+        <v>0</v>
+      </c>
+      <c r="S27" s="33">
+        <v>0</v>
+      </c>
+      <c r="T27" s="33">
+        <v>0</v>
+      </c>
+      <c r="U27" s="46">
+        <v>1</v>
+      </c>
+      <c r="V27" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="W27" s="45"/>
       <c r="X27" s="5"/>
     </row>
     <row r="28" spans="2:24">
       <c r="C28" s="1"/>
-      <c r="D28" s="9" t="s">
-        <v>22</v>
+      <c r="D28" s="80" t="s">
+        <v>103</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="8" t="s">
-        <v>113</v>
+      <c r="F28" s="79" t="s">
+        <v>102</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="54">
-        <v>11</v>
-      </c>
-      <c r="L28" s="43">
-        <v>0</v>
-      </c>
-      <c r="M28" s="44">
-        <v>0</v>
-      </c>
-      <c r="N28" s="37">
-        <v>0</v>
-      </c>
-      <c r="O28" s="38">
-        <v>0</v>
-      </c>
-      <c r="P28" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="38">
-        <v>0</v>
-      </c>
-      <c r="R28" s="38">
-        <v>0</v>
-      </c>
-      <c r="S28" s="38">
-        <v>0</v>
-      </c>
-      <c r="T28" s="38">
-        <v>0</v>
-      </c>
-      <c r="U28" s="50">
-        <v>0</v>
-      </c>
-      <c r="V28" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="W28" s="48"/>
+      <c r="K28" s="51">
+        <v>10</v>
+      </c>
+      <c r="L28" s="40">
+        <v>0</v>
+      </c>
+      <c r="M28" s="41">
+        <v>0</v>
+      </c>
+      <c r="N28" s="34">
+        <v>0</v>
+      </c>
+      <c r="O28" s="35">
+        <v>0</v>
+      </c>
+      <c r="P28" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="35">
+        <v>0</v>
+      </c>
+      <c r="R28" s="35">
+        <v>0</v>
+      </c>
+      <c r="S28" s="35">
+        <v>0</v>
+      </c>
+      <c r="T28" s="35">
+        <v>0</v>
+      </c>
+      <c r="U28" s="47">
+        <v>0</v>
+      </c>
+      <c r="V28" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="W28" s="45"/>
       <c r="X28" s="5"/>
     </row>
     <row r="29" spans="2:24">
       <c r="B29" s="1"/>
       <c r="C29" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="1"/>
       <c r="F29" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="I29" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J29" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="K29" s="54">
-        <v>12</v>
-      </c>
-      <c r="L29" s="43">
-        <v>0</v>
-      </c>
-      <c r="M29" s="44">
-        <v>0</v>
-      </c>
-      <c r="N29" s="37">
-        <v>0</v>
-      </c>
-      <c r="O29" s="38">
-        <v>0</v>
-      </c>
-      <c r="P29" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="38">
-        <v>0</v>
-      </c>
-      <c r="R29" s="38">
-        <v>0</v>
-      </c>
-      <c r="S29" s="38">
-        <v>0</v>
-      </c>
-      <c r="T29" s="38">
-        <v>0</v>
-      </c>
-      <c r="U29" s="50">
-        <v>0</v>
-      </c>
-      <c r="V29" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="W29" s="48"/>
+      <c r="I29" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="K29" s="51">
+        <v>11</v>
+      </c>
+      <c r="L29" s="40">
+        <v>0</v>
+      </c>
+      <c r="M29" s="41">
+        <v>0</v>
+      </c>
+      <c r="N29" s="34">
+        <v>0</v>
+      </c>
+      <c r="O29" s="35">
+        <v>0</v>
+      </c>
+      <c r="P29" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="35">
+        <v>0</v>
+      </c>
+      <c r="R29" s="35">
+        <v>0</v>
+      </c>
+      <c r="S29" s="35">
+        <v>0</v>
+      </c>
+      <c r="T29" s="35">
+        <v>0</v>
+      </c>
+      <c r="U29" s="47">
+        <v>0</v>
+      </c>
+      <c r="V29" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="W29" s="45"/>
       <c r="X29" s="5"/>
     </row>
     <row r="30" spans="2:24">
       <c r="B30" s="1"/>
-      <c r="C30" s="23"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="7"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="K30" s="54">
-        <v>16</v>
-      </c>
-      <c r="L30" s="43">
-        <v>0</v>
-      </c>
-      <c r="M30" s="44">
-        <v>1</v>
-      </c>
-      <c r="N30" s="37">
-        <v>0</v>
-      </c>
-      <c r="O30" s="38">
-        <v>0</v>
-      </c>
-      <c r="P30" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="38">
-        <v>0</v>
-      </c>
-      <c r="R30" s="38">
-        <v>0</v>
-      </c>
-      <c r="S30" s="38">
-        <v>1</v>
-      </c>
-      <c r="T30" s="38">
-        <v>0</v>
-      </c>
-      <c r="U30" s="50">
-        <v>0</v>
-      </c>
-      <c r="V30" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="W30" s="48"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="I30" s="23"/>
+      <c r="J30" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" s="51">
+        <v>12</v>
+      </c>
+      <c r="L30" s="40">
+        <v>0</v>
+      </c>
+      <c r="M30" s="41">
+        <v>0</v>
+      </c>
+      <c r="N30" s="34">
+        <v>0</v>
+      </c>
+      <c r="O30" s="35">
+        <v>0</v>
+      </c>
+      <c r="P30" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="35">
+        <v>0</v>
+      </c>
+      <c r="R30" s="35">
+        <v>0</v>
+      </c>
+      <c r="S30" s="35">
+        <v>0</v>
+      </c>
+      <c r="T30" s="35">
+        <v>0</v>
+      </c>
+      <c r="U30" s="47">
+        <v>0</v>
+      </c>
+      <c r="V30" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="W30" s="45"/>
       <c r="X30" s="5"/>
     </row>
     <row r="31" spans="2:24">
-      <c r="C31" s="7" t="s">
-        <v>55</v>
+      <c r="C31" s="76" t="s">
+        <v>95</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="56">
-        <v>17</v>
-      </c>
-      <c r="L31" s="45">
-        <v>0</v>
-      </c>
-      <c r="M31" s="46">
-        <v>0</v>
-      </c>
-      <c r="N31" s="39">
-        <v>0</v>
-      </c>
-      <c r="O31" s="40">
-        <v>0</v>
-      </c>
-      <c r="P31" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="40">
-        <v>0</v>
-      </c>
-      <c r="R31" s="40">
-        <v>0</v>
-      </c>
-      <c r="S31" s="40">
-        <v>0</v>
-      </c>
-      <c r="T31" s="40">
-        <v>0</v>
-      </c>
-      <c r="U31" s="51">
-        <v>0</v>
-      </c>
-      <c r="V31" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="W31" s="48"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="51">
+        <v>16</v>
+      </c>
+      <c r="L31" s="40">
+        <v>0</v>
+      </c>
+      <c r="M31" s="41">
+        <v>1</v>
+      </c>
+      <c r="N31" s="34">
+        <v>0</v>
+      </c>
+      <c r="O31" s="35">
+        <v>0</v>
+      </c>
+      <c r="P31" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="35">
+        <v>0</v>
+      </c>
+      <c r="R31" s="35">
+        <v>0</v>
+      </c>
+      <c r="S31" s="35">
+        <v>1</v>
+      </c>
+      <c r="T31" s="35">
+        <v>0</v>
+      </c>
+      <c r="U31" s="47">
+        <v>0</v>
+      </c>
+      <c r="V31" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="W31" s="45"/>
       <c r="X31" s="5"/>
     </row>
     <row r="32" spans="2:24">
-      <c r="C32" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K32" s="4"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="22"/>
+      <c r="C32" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="K32" s="53">
+        <v>17</v>
+      </c>
+      <c r="L32" s="42">
+        <v>0</v>
+      </c>
+      <c r="M32" s="43">
+        <v>0</v>
+      </c>
+      <c r="N32" s="36">
+        <v>0</v>
+      </c>
+      <c r="O32" s="37">
+        <v>0</v>
+      </c>
+      <c r="P32" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="37">
+        <v>0</v>
+      </c>
+      <c r="R32" s="37">
+        <v>0</v>
+      </c>
+      <c r="S32" s="37">
+        <v>0</v>
+      </c>
+      <c r="T32" s="37">
+        <v>0</v>
+      </c>
+      <c r="U32" s="48">
+        <v>0</v>
+      </c>
+      <c r="V32" s="54" t="s">
+        <v>76</v>
+      </c>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
     </row>
     <row r="33" spans="3:23">
-      <c r="C33" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>25</v>
+      <c r="C33" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="79" t="s">
+        <v>23</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="5"/>
@@ -7309,7 +8011,7 @@
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
-      <c r="V33" s="22"/>
+      <c r="V33" s="21"/>
       <c r="W33" s="5"/>
     </row>
     <row r="34" spans="3:23">
@@ -7326,17 +8028,17 @@
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
-      <c r="V34" s="22"/>
+      <c r="V34" s="21"/>
       <c r="W34" s="5"/>
     </row>
     <row r="35" spans="3:23">
       <c r="C35" s="8"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>85</v>
+      <c r="G35" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" s="78" t="s">
+        <v>65</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="5"/>
@@ -7349,12 +8051,12 @@
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
-      <c r="V35" s="22"/>
+      <c r="V35" s="21"/>
       <c r="W35" s="5"/>
     </row>
     <row r="36" spans="3:23">
       <c r="F36" s="11" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="5"/>
@@ -7367,17 +8069,17 @@
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
       <c r="U36" s="5"/>
-      <c r="V36" s="22"/>
+      <c r="V36" s="21"/>
       <c r="W36" s="5"/>
     </row>
     <row r="37" spans="3:23">
-      <c r="C37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="C37" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37" s="69" t="s">
         <v>15</v>
       </c>
       <c r="J37" s="1"/>
@@ -7395,19 +8097,19 @@
       <c r="V37" s="3"/>
     </row>
     <row r="38" spans="3:23">
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="79" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="I38" s="1" t="s">
-        <v>45</v>
+      <c r="I38" s="69" t="s">
+        <v>99</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="3:23">
       <c r="C39" s="8"/>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="75" t="s">
         <v>14</v>
       </c>
     </row>
@@ -7415,95 +8117,95 @@
       <c r="C40" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I40" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="J40" s="74"/>
-      <c r="K40" s="75"/>
+      <c r="E40" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="J40" s="84"/>
+      <c r="K40" s="85"/>
     </row>
     <row r="41" spans="3:23">
-      <c r="C41" s="1" t="s">
-        <v>49</v>
+      <c r="C41" s="69" t="s">
+        <v>113</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="F41" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>46</v>
+      <c r="F41" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="I41" s="69" t="s">
+        <v>112</v>
       </c>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="3:23">
       <c r="I42" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J42" s="21"/>
+        <v>19</v>
+      </c>
+      <c r="J42" s="20"/>
     </row>
     <row r="43" spans="3:23">
-      <c r="F43" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="F43" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
     </row>
     <row r="44" spans="3:23">
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
     </row>
     <row r="45" spans="3:23">
       <c r="F45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="N45" s="6"/>
     </row>
     <row r="46" spans="3:23">
-      <c r="F46" s="1" t="s">
-        <v>17</v>
+      <c r="F46" s="69" t="s">
+        <v>104</v>
       </c>
       <c r="L46" s="6"/>
       <c r="M46" s="6" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="3:23">
       <c r="J47" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K47" s="69">
+        <v>93</v>
+      </c>
+      <c r="K47" s="66">
         <v>3.5</v>
       </c>
       <c r="N47" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="3:23">
       <c r="C48" s="5"/>
-      <c r="D48" s="15"/>
+      <c r="D48" s="14"/>
       <c r="E48" s="5"/>
       <c r="F48" s="8"/>
       <c r="J48" t="s">
-        <v>71</v>
-      </c>
-      <c r="K48" s="32">
+        <v>53</v>
+      </c>
+      <c r="K48" s="29">
         <v>1.2</v>
       </c>
-      <c r="L48" s="33"/>
-      <c r="M48" s="32"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="29"/>
       <c r="N48" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="P48" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="3:25">
@@ -7511,114 +8213,110 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J49" t="s">
-        <v>111</v>
-      </c>
-      <c r="K49" s="70">
+        <v>86</v>
+      </c>
+      <c r="K49" s="67">
         <v>-0.5</v>
       </c>
-      <c r="L49" s="70"/>
-      <c r="M49" s="70"/>
+      <c r="L49" s="67"/>
+      <c r="M49" s="67"/>
       <c r="N49" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="P49" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="3:25">
-      <c r="C50" s="16"/>
-      <c r="D50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="14"/>
       <c r="E50" s="5"/>
-      <c r="F50" s="27" t="s">
-        <v>52</v>
+      <c r="F50" s="75" t="s">
+        <v>109</v>
       </c>
       <c r="G50" s="8"/>
       <c r="J50" t="s">
-        <v>68</v>
-      </c>
-      <c r="K50" s="69">
+        <v>50</v>
+      </c>
+      <c r="K50" s="66">
         <v>900</v>
       </c>
-      <c r="L50" s="69"/>
-      <c r="M50" s="69"/>
+      <c r="L50" s="66"/>
+      <c r="M50" s="66"/>
       <c r="N50" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="P50" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="V50" s="3"/>
     </row>
     <row r="51" spans="3:25">
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
       <c r="E51" s="5"/>
       <c r="J51" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K51" s="69">
+        <v>62</v>
+      </c>
+      <c r="K51" s="66">
         <v>1</v>
       </c>
-      <c r="L51" s="69"/>
-      <c r="M51" s="69"/>
+      <c r="L51" s="66"/>
+      <c r="M51" s="66"/>
       <c r="P51" s="3" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="3:25">
-      <c r="F52" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="P52" s="69"/>
-      <c r="Q52" s="69"/>
+      <c r="F52" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" s="71"/>
+      <c r="J52" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K52" s="66">
+        <v>1</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="53" spans="3:25">
-      <c r="F53" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="G53" s="72"/>
-      <c r="J53" t="s">
-        <v>18</v>
-      </c>
-      <c r="K53" s="69">
-        <v>4</v>
-      </c>
-      <c r="L53" s="69"/>
-      <c r="M53" s="69"/>
-      <c r="N53" t="s">
-        <v>76</v>
-      </c>
-      <c r="P53" t="s">
-        <v>73</v>
-      </c>
+      <c r="F53" s="81" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" s="82"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P53" s="66"/>
+      <c r="Q53" s="66"/>
     </row>
     <row r="54" spans="3:25">
-      <c r="F54" s="1" t="s">
-        <v>57</v>
+      <c r="F54" s="69" t="s">
+        <v>105</v>
       </c>
       <c r="J54" t="s">
-        <v>19</v>
-      </c>
-      <c r="K54" s="69">
-        <v>15</v>
-      </c>
-      <c r="L54" s="69"/>
-      <c r="M54" s="69"/>
+        <v>17</v>
+      </c>
+      <c r="K54" s="66">
+        <v>5</v>
+      </c>
+      <c r="L54" s="66"/>
+      <c r="M54" s="66"/>
       <c r="N54" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="P54" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
@@ -7626,53 +8324,59 @@
       <c r="U54" s="6"/>
     </row>
     <row r="55" spans="3:25">
+      <c r="F55" s="16" t="s">
+        <v>107</v>
+      </c>
       <c r="I55" s="3"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="34"/>
-      <c r="Q55" s="34"/>
+      <c r="J55" t="s">
+        <v>18</v>
+      </c>
+      <c r="K55" s="66">
+        <v>12</v>
+      </c>
+      <c r="L55" s="66"/>
+      <c r="M55" s="66"/>
+      <c r="N55" t="s">
+        <v>57</v>
+      </c>
+      <c r="P55" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="56" spans="3:25">
+      <c r="D56" s="16" t="s">
+        <v>108</v>
+      </c>
       <c r="F56" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G56" s="18"/>
-      <c r="J56" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="K56" s="76">
-        <v>50</v>
-      </c>
-      <c r="N56" t="s">
-        <v>70</v>
-      </c>
-      <c r="P56" s="3" t="s">
-        <v>118</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="31"/>
+      <c r="Q56" s="31"/>
     </row>
     <row r="57" spans="3:25">
-      <c r="F57" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="J57" t="s">
-        <v>77</v>
-      </c>
-      <c r="K57" s="69">
-        <v>120</v>
-      </c>
-      <c r="L57" s="69"/>
-      <c r="M57" s="69"/>
+      <c r="F57" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K57" s="68">
+        <v>50</v>
+      </c>
       <c r="N57" t="s">
-        <v>75</v>
-      </c>
-      <c r="P57" t="s">
-        <v>93</v>
+        <v>52</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="V57" s="6"/>
       <c r="W57" s="6"/>
@@ -7680,54 +8384,90 @@
       <c r="Y57" s="6"/>
     </row>
     <row r="58" spans="3:25">
-      <c r="F58" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K58" s="69">
-        <v>95</v>
-      </c>
-      <c r="L58" s="69"/>
-      <c r="M58" s="69"/>
+      <c r="F58" s="78"/>
+      <c r="J58" t="s">
+        <v>59</v>
+      </c>
+      <c r="K58" s="66">
+        <v>120</v>
+      </c>
+      <c r="L58" s="66"/>
+      <c r="M58" s="66"/>
       <c r="N58" t="s">
-        <v>70</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>91</v>
+        <v>57</v>
+      </c>
+      <c r="P58" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="3:25">
-      <c r="F59" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="G59" s="72"/>
+      <c r="F59" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="G59" s="82"/>
       <c r="J59" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K59" s="69">
-        <v>105</v>
-      </c>
-      <c r="L59" s="69"/>
-      <c r="M59" s="69"/>
+        <v>63</v>
+      </c>
+      <c r="K59" s="66">
+        <v>95</v>
+      </c>
+      <c r="L59" s="66"/>
+      <c r="M59" s="66"/>
       <c r="N59" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="P59" s="3" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="V59" s="3"/>
     </row>
     <row r="60" spans="3:25">
-      <c r="F60" s="28" t="s">
-        <v>54</v>
+      <c r="F60" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K60" s="66">
+        <v>105</v>
+      </c>
+      <c r="L60" s="66"/>
+      <c r="M60" s="66"/>
+      <c r="N60" t="s">
+        <v>52</v>
+      </c>
+      <c r="P60" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="V60" s="3"/>
+    </row>
+    <row r="61" spans="3:25">
+      <c r="J61" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K61" s="66">
+        <v>1</v>
+      </c>
+      <c r="N61" s="3"/>
+      <c r="P61" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="62" spans="3:25">
       <c r="F62" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="K62" s="66">
+        <v>98.5</v>
+      </c>
+      <c r="N62" t="s">
+        <v>52</v>
+      </c>
+      <c r="P62" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="5:6">
@@ -7745,8 +8485,8 @@
     <mergeCell ref="I40:K40"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.4" right="0.37" top="0.21" bottom="0.38" header="0.28000000000000003" footer="0.3"/>
-  <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.35433070866141736" top="0.19685039370078741" bottom="0.39370078740157483" header="0.27559055118110237" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>